<commit_message>
Updated packet_def and packet_apid file for adcs_css
</commit_message>
<xml_diff>
--- a/is_1_handbook.xlsx
+++ b/is_1_handbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anant\PycharmProjects\IS1_Temeletry_Decoding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF43070-59D4-445D-AE09-1DED817565FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED4AF08-09D1-4B58-A790-7936226BD906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="5310" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inspire_pkt" sheetId="1" r:id="rId1"/>
@@ -12174,12 +12174,19 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C6" sqref="A1:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -13124,8 +13131,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q1780"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A804" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B804" sqref="B804"/>
+    <sheetView tabSelected="1" topLeftCell="A1421" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F1437" sqref="F1437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30934,7 +30941,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="770" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>1277</v>
       </c>
@@ -30954,7 +30961,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="771" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="771" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
         <v>1277</v>
       </c>
@@ -30974,7 +30981,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="772" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
         <v>1277</v>
       </c>
@@ -30994,7 +31001,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="773" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>1277</v>
       </c>
@@ -31014,7 +31021,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="774" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
         <v>1277</v>
       </c>
@@ -31034,7 +31041,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="775" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
         <v>1277</v>
       </c>
@@ -31054,7 +31061,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="776" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>1277</v>
       </c>
@@ -31074,7 +31081,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="777" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
         <v>1277</v>
       </c>
@@ -31100,7 +31107,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="778" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
         <v>1277</v>
       </c>
@@ -31126,7 +31133,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="779" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
         <v>73</v>
       </c>
@@ -31149,7 +31156,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="780" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
         <v>73</v>
       </c>
@@ -31172,7 +31179,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="781" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
         <v>73</v>
       </c>
@@ -31198,7 +31205,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="782" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
         <v>73</v>
       </c>
@@ -31224,7 +31231,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="783" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
         <v>73</v>
       </c>
@@ -31250,7 +31257,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="784" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
         <v>73</v>
       </c>
@@ -31276,7 +31283,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="785" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
         <v>73</v>
       </c>
@@ -31302,7 +31309,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="786" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
         <v>73</v>
       </c>
@@ -31328,7 +31335,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="787" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
         <v>73</v>
       </c>
@@ -31354,7 +31361,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="788" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
         <v>73</v>
       </c>
@@ -31380,7 +31387,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="789" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
         <v>73</v>
       </c>
@@ -31406,7 +31413,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="790" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
         <v>73</v>
       </c>
@@ -31432,7 +31439,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="791" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
         <v>73</v>
       </c>
@@ -31458,7 +31465,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="792" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
         <v>73</v>
       </c>
@@ -31484,7 +31491,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="793" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
         <v>73</v>
       </c>
@@ -31510,7 +31517,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="794" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
         <v>73</v>
       </c>
@@ -31536,7 +31543,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="795" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
         <v>73</v>
       </c>
@@ -31562,7 +31569,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="796" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
         <v>73</v>
       </c>
@@ -31588,7 +31595,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="797" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
         <v>73</v>
       </c>
@@ -31614,7 +31621,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="798" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
         <v>73</v>
       </c>
@@ -31640,7 +31647,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="799" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
         <v>73</v>
       </c>
@@ -31666,7 +31673,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="800" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
         <v>73</v>
       </c>
@@ -31692,7 +31699,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="801" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
         <v>73</v>
       </c>
@@ -31718,7 +31725,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="802" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
         <v>73</v>
       </c>
@@ -31744,7 +31751,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="803" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
         <v>73</v>
       </c>
@@ -31770,7 +31777,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="804" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
         <v>73</v>
       </c>
@@ -31796,7 +31803,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="805" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
         <v>73</v>
       </c>
@@ -31822,7 +31829,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="806" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
         <v>73</v>
       </c>
@@ -31848,7 +31855,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="807" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
         <v>73</v>
       </c>
@@ -31874,7 +31881,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="808" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
         <v>73</v>
       </c>
@@ -31900,7 +31907,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="809" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
         <v>73</v>
       </c>
@@ -31926,7 +31933,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="810" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
         <v>73</v>
       </c>
@@ -31952,7 +31959,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="811" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
         <v>73</v>
       </c>
@@ -31978,7 +31985,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="812" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
         <v>73</v>
       </c>
@@ -32004,7 +32011,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="813" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
         <v>73</v>
       </c>
@@ -32030,7 +32037,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="814" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
         <v>73</v>
       </c>
@@ -32056,7 +32063,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="815" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
         <v>73</v>
       </c>
@@ -32082,7 +32089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="816" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
         <v>73</v>
       </c>
@@ -32108,7 +32115,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="817" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
         <v>73</v>
       </c>
@@ -32134,7 +32141,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="818" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
         <v>73</v>
       </c>
@@ -32157,7 +32164,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="819" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
         <v>73</v>
       </c>
@@ -32183,7 +32190,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="820" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
         <v>73</v>
       </c>
@@ -32209,7 +32216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="821" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
         <v>73</v>
       </c>
@@ -32235,7 +32242,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="822" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
         <v>73</v>
       </c>
@@ -32261,7 +32268,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="823" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
         <v>73</v>
       </c>
@@ -32287,7 +32294,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="824" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
         <v>466</v>
       </c>
@@ -32304,7 +32311,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="825" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
         <v>496</v>
       </c>
@@ -32321,7 +32328,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="826" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
         <v>534</v>
       </c>
@@ -45916,7 +45923,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1400" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1400" t="s">
         <v>533</v>
       </c>
@@ -45936,7 +45943,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1401" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1401" t="s">
         <v>533</v>
       </c>
@@ -45956,7 +45963,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1402" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1402" t="s">
         <v>533</v>
       </c>
@@ -45976,7 +45983,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1403" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1403" t="s">
         <v>533</v>
       </c>
@@ -45996,7 +46003,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1404" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1404" t="s">
         <v>533</v>
       </c>
@@ -46016,7 +46023,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1405" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1405" t="s">
         <v>533</v>
       </c>
@@ -46036,7 +46043,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1406" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1406" t="s">
         <v>533</v>
       </c>
@@ -46056,7 +46063,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1407" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1407" t="s">
         <v>533</v>
       </c>
@@ -46082,7 +46089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1408" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1408" t="s">
         <v>533</v>
       </c>
@@ -46108,7 +46115,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1409" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1409" t="s">
         <v>73</v>
       </c>
@@ -46134,7 +46141,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1410" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1410" t="s">
         <v>73</v>
       </c>
@@ -46160,7 +46167,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1411" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1411" t="s">
         <v>73</v>
       </c>
@@ -46186,7 +46193,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1412" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1412" t="s">
         <v>73</v>
       </c>
@@ -46212,7 +46219,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1413" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1413" t="s">
         <v>73</v>
       </c>
@@ -46235,7 +46242,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1414" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1414" t="s">
         <v>73</v>
       </c>
@@ -46258,7 +46265,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1415" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1415" t="s">
         <v>73</v>
       </c>
@@ -46281,7 +46288,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1416" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1416" t="s">
         <v>73</v>
       </c>
@@ -46304,7 +46311,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1417" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1417" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1417" t="s">
         <v>73</v>
       </c>
@@ -46327,7 +46334,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1418" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1418" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1418" t="s">
         <v>73</v>
       </c>
@@ -46350,7 +46357,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1419" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1419" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1419" t="s">
         <v>73</v>
       </c>
@@ -46373,7 +46380,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1420" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1420" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1420" t="s">
         <v>73</v>
       </c>
@@ -46396,7 +46403,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1421" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1421" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1421" t="s">
         <v>73</v>
       </c>
@@ -46419,7 +46426,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1422" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1422" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1422" t="s">
         <v>73</v>
       </c>
@@ -46442,7 +46449,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1423" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1423" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1423" t="s">
         <v>73</v>
       </c>
@@ -46465,7 +46472,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1424" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1424" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1424" t="s">
         <v>73</v>
       </c>
@@ -46488,7 +46495,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1425" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1425" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1425" t="s">
         <v>73</v>
       </c>
@@ -46511,7 +46518,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1426" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1426" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1426" t="s">
         <v>73</v>
       </c>
@@ -46534,7 +46541,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1427" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1427" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1427" t="s">
         <v>73</v>
       </c>
@@ -46557,7 +46564,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1428" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1428" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1428" t="s">
         <v>73</v>
       </c>
@@ -46580,7 +46587,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1429" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1429" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1429" t="s">
         <v>73</v>
       </c>
@@ -46603,7 +46610,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1430" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1430" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1430" t="s">
         <v>73</v>
       </c>
@@ -46626,7 +46633,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1431" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1431" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1431" t="s">
         <v>73</v>
       </c>
@@ -46649,7 +46656,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1432" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1432" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1432" t="s">
         <v>73</v>
       </c>
@@ -46672,7 +46679,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1433" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1433" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1433" t="s">
         <v>73</v>
       </c>
@@ -46698,7 +46705,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1434" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1434" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1434" t="s">
         <v>73</v>
       </c>
@@ -46721,7 +46728,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1435" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1435" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1435" t="s">
         <v>73</v>
       </c>
@@ -46747,7 +46754,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1436" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1436" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1436" t="s">
         <v>466</v>
       </c>
@@ -46764,7 +46771,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="1437" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1437" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1437" t="s">
         <v>496</v>
       </c>
@@ -54638,7 +54645,7 @@
   <autoFilter ref="A1:Q1780" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="adcs_refs"/>
+        <filter val="adcs_css"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>